<commit_message>
Test Past of Full Run of the following lipids: - PC [M+HCOO]+ - LPC [M+HCOO]+ - PE [M-H]- - LPE [M-H]- - PS [M-H]- - PG [M-H]- - PI [M-H]- - DG [M+NH4]+ - TG [M+NH4]+ - Cer [M+H]+
Issues:
- 1 core not running from interface but running from Hunter_Core.py
- Ceramides output needs to double check
- Weight List need to be double checked for ceramides
- Integrated the ceramide inside the interface
</commit_message>
<xml_diff>
--- a/ConfigurationFiles/1-FA_Whitelist.xlsx
+++ b/ConfigurationFiles/1-FA_Whitelist.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="108">
   <si>
     <t>FattyAcid</t>
   </si>
@@ -256,6 +256,93 @@
   </si>
   <si>
     <t>PL</t>
+  </si>
+  <si>
+    <t>SPB16:0;1</t>
+  </si>
+  <si>
+    <t>SPB16:0;2</t>
+  </si>
+  <si>
+    <t>SPB16:0;3</t>
+  </si>
+  <si>
+    <t>SPB16:1;2</t>
+  </si>
+  <si>
+    <t>SPB16:1;3</t>
+  </si>
+  <si>
+    <t>SPB17:0;1</t>
+  </si>
+  <si>
+    <t>SPB17:0;2</t>
+  </si>
+  <si>
+    <t>SPB17:0;3</t>
+  </si>
+  <si>
+    <t>SPB17:1;1</t>
+  </si>
+  <si>
+    <t>SPB17:1;2</t>
+  </si>
+  <si>
+    <t>SPB17:1;3</t>
+  </si>
+  <si>
+    <t>SPB18:0;1</t>
+  </si>
+  <si>
+    <t>SPB18:0;3</t>
+  </si>
+  <si>
+    <t>SPB18:1;1</t>
+  </si>
+  <si>
+    <t>SPB18:1;3</t>
+  </si>
+  <si>
+    <t>SPB19:0;1</t>
+  </si>
+  <si>
+    <t>SPB19:0;2</t>
+  </si>
+  <si>
+    <t>SPB19:0;3</t>
+  </si>
+  <si>
+    <t>SPB19:1;1</t>
+  </si>
+  <si>
+    <t>SPB19:1;2</t>
+  </si>
+  <si>
+    <t>SPB19:1;3</t>
+  </si>
+  <si>
+    <t>SPB20:0;1</t>
+  </si>
+  <si>
+    <t>SPB20:0;2</t>
+  </si>
+  <si>
+    <t>SPB20:1;1</t>
+  </si>
+  <si>
+    <t>SPB20:1;2</t>
+  </si>
+  <si>
+    <t>SPB20:1;3</t>
+  </si>
+  <si>
+    <t>SPB18:2;1</t>
+  </si>
+  <si>
+    <t>SPB18:2;2</t>
+  </si>
+  <si>
+    <t>FA21:0</t>
   </si>
 </sst>
 </file>
@@ -573,10 +660,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I70"/>
+  <dimension ref="A1:I99"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Q29" sqref="Q29"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="I41" sqref="I41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -638,6 +725,9 @@
       <c r="H2" t="s">
         <v>18</v>
       </c>
+      <c r="I2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
@@ -664,6 +754,9 @@
       <c r="H3" t="s">
         <v>18</v>
       </c>
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
@@ -690,6 +783,9 @@
       <c r="H4" t="s">
         <v>18</v>
       </c>
+      <c r="I4" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
@@ -716,6 +812,9 @@
       <c r="H5" t="s">
         <v>18</v>
       </c>
+      <c r="I5" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
@@ -742,6 +841,9 @@
       <c r="H6" t="s">
         <v>18</v>
       </c>
+      <c r="I6" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
@@ -768,6 +870,9 @@
       <c r="H7" t="s">
         <v>18</v>
       </c>
+      <c r="I7" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
@@ -794,6 +899,9 @@
       <c r="H8" t="s">
         <v>18</v>
       </c>
+      <c r="I8" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
@@ -820,6 +928,9 @@
       <c r="H9" t="s">
         <v>18</v>
       </c>
+      <c r="I9" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
@@ -846,6 +957,9 @@
       <c r="H10" t="s">
         <v>18</v>
       </c>
+      <c r="I10" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
@@ -872,6 +986,9 @@
       <c r="H11" t="s">
         <v>18</v>
       </c>
+      <c r="I11" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
@@ -898,6 +1015,9 @@
       <c r="H12" t="s">
         <v>18</v>
       </c>
+      <c r="I12" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
@@ -924,6 +1044,9 @@
       <c r="H13" t="s">
         <v>18</v>
       </c>
+      <c r="I13" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
@@ -950,6 +1073,9 @@
       <c r="H14" t="s">
         <v>18</v>
       </c>
+      <c r="I14" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
@@ -1707,27 +1833,12 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
-        <v>24</v>
+        <v>107</v>
       </c>
       <c r="B41" t="s">
         <v>18</v>
       </c>
       <c r="C41" t="s">
-        <v>18</v>
-      </c>
-      <c r="D41" t="s">
-        <v>18</v>
-      </c>
-      <c r="E41" t="s">
-        <v>18</v>
-      </c>
-      <c r="F41" t="s">
-        <v>18</v>
-      </c>
-      <c r="G41" t="s">
-        <v>18</v>
-      </c>
-      <c r="H41" t="s">
         <v>18</v>
       </c>
       <c r="I41" t="s">
@@ -1736,7 +1847,7 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A42" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B42" t="s">
         <v>18</v>
@@ -1765,7 +1876,7 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B43" t="s">
         <v>18</v>
@@ -1794,7 +1905,7 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A44" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B44" t="s">
         <v>18</v>
@@ -1823,7 +1934,7 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A45" t="s">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="B45" t="s">
         <v>18</v>
@@ -1852,7 +1963,7 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A46" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B46" t="s">
         <v>18</v>
@@ -1881,7 +1992,7 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A47" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B47" t="s">
         <v>18</v>
@@ -1899,6 +2010,9 @@
         <v>18</v>
       </c>
       <c r="G47" t="s">
+        <v>18</v>
+      </c>
+      <c r="H47" t="s">
         <v>18</v>
       </c>
       <c r="I47" t="s">
@@ -1907,7 +2021,7 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A48" t="s">
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="B48" t="s">
         <v>18</v>
@@ -1925,6 +2039,9 @@
         <v>18</v>
       </c>
       <c r="G48" t="s">
+        <v>18</v>
+      </c>
+      <c r="H48" t="s">
         <v>18</v>
       </c>
       <c r="I48" t="s">
@@ -1933,9 +2050,27 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A49" t="s">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="B49" t="s">
+        <v>18</v>
+      </c>
+      <c r="C49" t="s">
+        <v>18</v>
+      </c>
+      <c r="D49" t="s">
+        <v>18</v>
+      </c>
+      <c r="E49" t="s">
+        <v>18</v>
+      </c>
+      <c r="F49" t="s">
+        <v>18</v>
+      </c>
+      <c r="G49" t="s">
+        <v>18</v>
+      </c>
+      <c r="H49" t="s">
         <v>18</v>
       </c>
       <c r="I49" t="s">
@@ -1944,9 +2079,12 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A50" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B50" t="s">
+        <v>18</v>
+      </c>
+      <c r="H50" t="s">
         <v>18</v>
       </c>
       <c r="I50" t="s">
@@ -1955,24 +2093,12 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A51" t="s">
-        <v>25</v>
+        <v>71</v>
       </c>
       <c r="B51" t="s">
         <v>18</v>
       </c>
-      <c r="C51" t="s">
-        <v>18</v>
-      </c>
-      <c r="D51" t="s">
-        <v>18</v>
-      </c>
-      <c r="E51" t="s">
-        <v>18</v>
-      </c>
-      <c r="F51" t="s">
-        <v>18</v>
-      </c>
-      <c r="G51" t="s">
+      <c r="H51" t="s">
         <v>18</v>
       </c>
       <c r="I51" t="s">
@@ -1981,7 +2107,7 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A52" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="B52" t="s">
         <v>18</v>
@@ -1999,6 +2125,9 @@
         <v>18</v>
       </c>
       <c r="G52" t="s">
+        <v>18</v>
+      </c>
+      <c r="H52" t="s">
         <v>18</v>
       </c>
       <c r="I52" t="s">
@@ -2007,7 +2136,7 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A53" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B53" t="s">
         <v>18</v>
@@ -2025,6 +2154,9 @@
         <v>18</v>
       </c>
       <c r="G53" t="s">
+        <v>18</v>
+      </c>
+      <c r="H53" t="s">
         <v>18</v>
       </c>
       <c r="I53" t="s">
@@ -2033,7 +2165,7 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A54" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B54" t="s">
         <v>18</v>
@@ -2051,6 +2183,9 @@
         <v>18</v>
       </c>
       <c r="G54" t="s">
+        <v>18</v>
+      </c>
+      <c r="H54" t="s">
         <v>18</v>
       </c>
       <c r="I54" t="s">
@@ -2059,7 +2194,7 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A55" t="s">
-        <v>67</v>
+        <v>37</v>
       </c>
       <c r="B55" t="s">
         <v>18</v>
@@ -2077,6 +2212,9 @@
         <v>18</v>
       </c>
       <c r="G55" t="s">
+        <v>18</v>
+      </c>
+      <c r="H55" t="s">
         <v>18</v>
       </c>
       <c r="I55" t="s">
@@ -2085,9 +2223,27 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A56" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B56" t="s">
+        <v>18</v>
+      </c>
+      <c r="C56" t="s">
+        <v>18</v>
+      </c>
+      <c r="D56" t="s">
+        <v>18</v>
+      </c>
+      <c r="E56" t="s">
+        <v>18</v>
+      </c>
+      <c r="F56" t="s">
+        <v>18</v>
+      </c>
+      <c r="G56" t="s">
+        <v>18</v>
+      </c>
+      <c r="H56" t="s">
         <v>18</v>
       </c>
       <c r="I56" t="s">
@@ -2096,9 +2252,12 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A57" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B57" t="s">
+        <v>18</v>
+      </c>
+      <c r="H57" t="s">
         <v>18</v>
       </c>
       <c r="I57" t="s">
@@ -2107,24 +2266,12 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A58" t="s">
-        <v>26</v>
+        <v>73</v>
       </c>
       <c r="B58" t="s">
         <v>18</v>
       </c>
-      <c r="C58" t="s">
-        <v>18</v>
-      </c>
-      <c r="D58" t="s">
-        <v>18</v>
-      </c>
-      <c r="E58" t="s">
-        <v>18</v>
-      </c>
-      <c r="F58" t="s">
-        <v>18</v>
-      </c>
-      <c r="G58" t="s">
+      <c r="H58" t="s">
         <v>18</v>
       </c>
       <c r="I58" t="s">
@@ -2133,7 +2280,7 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A59" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="B59" t="s">
         <v>18</v>
@@ -2151,12 +2298,18 @@
         <v>18</v>
       </c>
       <c r="G59" t="s">
+        <v>18</v>
+      </c>
+      <c r="H59" t="s">
+        <v>18</v>
+      </c>
+      <c r="I59" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A60" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B60" t="s">
         <v>18</v>
@@ -2174,16 +2327,28 @@
         <v>18</v>
       </c>
       <c r="G60" t="s">
+        <v>18</v>
+      </c>
+      <c r="H60" t="s">
+        <v>18</v>
+      </c>
+      <c r="I60" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A61" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
       <c r="B61" t="s">
         <v>18</v>
       </c>
+      <c r="C61" t="s">
+        <v>18</v>
+      </c>
+      <c r="D61" t="s">
+        <v>18</v>
+      </c>
       <c r="E61" t="s">
         <v>18</v>
       </c>
@@ -2191,12 +2356,15 @@
         <v>18</v>
       </c>
       <c r="G61" t="s">
+        <v>18</v>
+      </c>
+      <c r="I61" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A62" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B62" t="s">
         <v>18</v>
@@ -2213,7 +2381,7 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A63" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B63" t="s">
         <v>18</v>
@@ -2230,7 +2398,7 @@
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A64" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B64" t="s">
         <v>18</v>
@@ -2247,7 +2415,7 @@
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A65" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B65" t="s">
         <v>18</v>
@@ -2264,7 +2432,7 @@
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A66" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B66" t="s">
         <v>18</v>
@@ -2281,36 +2449,370 @@
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A67" t="s">
-        <v>74</v>
+        <v>17</v>
       </c>
       <c r="B67" t="s">
         <v>18</v>
       </c>
-      <c r="I67" t="s">
+      <c r="E67" t="s">
+        <v>18</v>
+      </c>
+      <c r="F67" t="s">
+        <v>18</v>
+      </c>
+      <c r="G67" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A68" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B68" t="s">
+        <v>18</v>
+      </c>
+      <c r="I68" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A69" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B69" t="s">
+        <v>18</v>
+      </c>
+      <c r="I69" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A70" t="s">
+        <v>84</v>
+      </c>
+      <c r="B70" t="s">
+        <v>18</v>
+      </c>
+      <c r="I70" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A71" t="s">
+        <v>87</v>
+      </c>
+      <c r="B71" t="s">
+        <v>18</v>
+      </c>
+      <c r="I71" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A72" t="s">
+        <v>90</v>
+      </c>
+      <c r="B72" t="s">
+        <v>18</v>
+      </c>
+      <c r="I72" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A73" t="s">
+        <v>92</v>
+      </c>
+      <c r="B73" t="s">
+        <v>18</v>
+      </c>
+      <c r="I73" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A74" t="s">
+        <v>105</v>
+      </c>
+      <c r="B74" t="s">
+        <v>18</v>
+      </c>
+      <c r="I74" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A75" t="s">
+        <v>94</v>
+      </c>
+      <c r="B75" t="s">
+        <v>18</v>
+      </c>
+      <c r="I75" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A76" t="s">
+        <v>97</v>
+      </c>
+      <c r="B76" t="s">
+        <v>18</v>
+      </c>
+      <c r="I76" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A77" t="s">
+        <v>100</v>
+      </c>
+      <c r="B77" t="s">
+        <v>18</v>
+      </c>
+      <c r="I77" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A78" t="s">
+        <v>102</v>
+      </c>
+      <c r="B78" t="s">
+        <v>18</v>
+      </c>
+      <c r="I78" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A79" t="s">
+        <v>80</v>
+      </c>
+      <c r="B79" t="s">
+        <v>18</v>
+      </c>
+      <c r="I79" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A80" t="s">
+        <v>82</v>
+      </c>
+      <c r="B80" t="s">
+        <v>18</v>
+      </c>
+      <c r="I80" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A81" t="s">
+        <v>85</v>
+      </c>
+      <c r="B81" t="s">
+        <v>18</v>
+      </c>
+      <c r="I81" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A82" t="s">
+        <v>88</v>
+      </c>
+      <c r="B82" t="s">
+        <v>18</v>
+      </c>
+      <c r="I82" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A83" t="s">
+        <v>75</v>
+      </c>
+      <c r="B83" t="s">
+        <v>18</v>
+      </c>
+      <c r="I83" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A84" t="s">
+        <v>74</v>
+      </c>
+      <c r="B84" t="s">
+        <v>18</v>
+      </c>
+      <c r="I84" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A85" t="s">
+        <v>106</v>
+      </c>
+      <c r="B85" t="s">
+        <v>18</v>
+      </c>
+      <c r="I85" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A86" t="s">
+        <v>95</v>
+      </c>
+      <c r="B86" t="s">
+        <v>18</v>
+      </c>
+      <c r="I86" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A87" t="s">
+        <v>98</v>
+      </c>
+      <c r="B87" t="s">
+        <v>18</v>
+      </c>
+      <c r="I87" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A88" t="s">
+        <v>101</v>
+      </c>
+      <c r="B88" t="s">
+        <v>18</v>
+      </c>
+      <c r="I88" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A89" t="s">
+        <v>103</v>
+      </c>
+      <c r="B89" t="s">
+        <v>18</v>
+      </c>
+      <c r="I89" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A90" t="s">
+        <v>81</v>
+      </c>
+      <c r="B90" t="s">
+        <v>18</v>
+      </c>
+      <c r="I90" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A91" t="s">
+        <v>83</v>
+      </c>
+      <c r="B91" t="s">
+        <v>18</v>
+      </c>
+      <c r="I91" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A92" t="s">
+        <v>86</v>
+      </c>
+      <c r="B92" t="s">
+        <v>18</v>
+      </c>
+      <c r="I92" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A93" t="s">
+        <v>89</v>
+      </c>
+      <c r="B93" t="s">
+        <v>18</v>
+      </c>
+      <c r="I93" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A94" t="s">
+        <v>91</v>
+      </c>
+      <c r="B94" t="s">
+        <v>18</v>
+      </c>
+      <c r="I94" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A95" t="s">
+        <v>93</v>
+      </c>
+      <c r="B95" t="s">
+        <v>18</v>
+      </c>
+      <c r="I95" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A96" t="s">
+        <v>96</v>
+      </c>
+      <c r="B96" t="s">
+        <v>18</v>
+      </c>
+      <c r="I96" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A97" t="s">
+        <v>99</v>
+      </c>
+      <c r="B97" t="s">
+        <v>18</v>
+      </c>
+      <c r="I97" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A98" t="s">
         <v>77</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B98" t="s">
+        <v>18</v>
+      </c>
+      <c r="I98" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A99" t="s">
+        <v>104</v>
+      </c>
+      <c r="B99" t="s">
+        <v>18</v>
+      </c>
+      <c r="I99" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Change the Weight Score for Ceramides: Instead of a one common one is split in 3. Each group of SPB (m, d, t) has different Weight score which will be use to calculate the rank score
</commit_message>
<xml_diff>
--- a/ConfigurationFiles/1-FA_Whitelist.xlsx
+++ b/ConfigurationFiles/1-FA_Whitelist.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="109">
   <si>
     <t>FattyAcid</t>
   </si>
@@ -343,6 +343,9 @@
   </si>
   <si>
     <t>FA21:0</t>
+  </si>
+  <si>
+    <t>SPB15:0;1</t>
   </si>
 </sst>
 </file>
@@ -660,10 +663,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I99"/>
+  <dimension ref="A1:I100"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="I41" sqref="I41"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -2257,6 +2260,9 @@
       <c r="B57" t="s">
         <v>18</v>
       </c>
+      <c r="C57" t="s">
+        <v>18</v>
+      </c>
       <c r="H57" t="s">
         <v>18</v>
       </c>
@@ -2271,6 +2277,9 @@
       <c r="B58" t="s">
         <v>18</v>
       </c>
+      <c r="C58" t="s">
+        <v>18</v>
+      </c>
       <c r="H58" t="s">
         <v>18</v>
       </c>
@@ -2813,6 +2822,17 @@
         <v>18</v>
       </c>
       <c r="I99" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A100" t="s">
+        <v>108</v>
+      </c>
+      <c r="B100" t="s">
+        <v>18</v>
+      </c>
+      <c r="I100" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>